<commit_message>
Change Mesh Sailor & Monkey
</commit_message>
<xml_diff>
--- a/The Eternals/FrameDirectX12/Bin/Resource/ResourceStage/DynamicMesh/Monster/DrownedSailor/AnimationInfo.xlsx
+++ b/The Eternals/FrameDirectX12/Bin/Resource/ResourceStage/DynamicMesh/Monster/DrownedSailor/AnimationInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\01.KPUFinalProject\The Eternals\FrameDirectX12\Bin\Resource\ResourceStage\DynamicMesh\Monster\DrownedSailor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08020B3-A02B-4AE9-BA31-EBC4FF37CB6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B879B7D0-0F50-4C98-9269-933DAAAFF1C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21770" yWindow="0" windowWidth="14070" windowHeight="10400" xr2:uid="{61396BBF-947E-42B3-B422-339E63356C45}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61396BBF-947E-42B3-B422-339E63356C45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Animation Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>attack6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groggy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>knockback</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -484,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3945F1B-935D-41F2-9305-F8AE345AF27E}">
-  <dimension ref="C3:F12"/>
+  <dimension ref="C3:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -635,6 +647,48 @@
         <v>588</v>
       </c>
     </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>589</v>
+      </c>
+      <c r="F13" s="1">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <v>620</v>
+      </c>
+      <c r="F14" s="1">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
+        <v>669</v>
+      </c>
+      <c r="F15" s="1">
+        <v>807</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>